<commit_message>
Added new colums to report, adjusted readme and included option to select date range. Also added xlsx template for Excel reports
</commit_message>
<xml_diff>
--- a/reports/active_assets/templates/xlsx/template.xlsx
+++ b/reports/active_assets/templates/xlsx/template.xlsx
@@ -1,34 +1,133 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idigon/Repos/adobe_connect_reports/reports/active_assets/templates/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F449CF8-2CD8-E048-ADE9-EFBF944F8DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>Asset Status</t>
+  </si>
+  <si>
+    <t>Asset Id</t>
+  </si>
+  <si>
+    <t>External Id</t>
+  </si>
+  <si>
+    <t>Product Id</t>
+  </si>
+  <si>
+    <t>Provider Id</t>
+  </si>
+  <si>
+    <t>Provider Name</t>
+  </si>
+  <si>
+    <t>Marketplace Id</t>
+  </si>
+  <si>
+    <t>Marketplace Name</t>
+  </si>
+  <si>
+    <t>Contract Id</t>
+  </si>
+  <si>
+    <t>Contract Name</t>
+  </si>
+  <si>
+    <t>Reseller Id</t>
+  </si>
+  <si>
+    <t>Reseller External Id</t>
+  </si>
+  <si>
+    <t>Reseller Name</t>
+  </si>
+  <si>
+    <t>Created At</t>
+  </si>
+  <si>
+    <t>Customer Id</t>
+  </si>
+  <si>
+    <t>Customer External Id</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Seamless Move</t>
+  </si>
+  <si>
+    <t>Discount Group</t>
+  </si>
+  <si>
+    <t>Renewal Date</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>PurchaseType</t>
+  </si>
+  <si>
+    <t>Adobe Customer Id</t>
+  </si>
+  <si>
+    <t>Adobe VIP Number</t>
+  </si>
+  <si>
+    <t>Adobe User Email</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>MSRP</t>
+  </si>
+  <si>
+    <t>Reseller Cost</t>
+  </si>
+  <si>
+    <t>Seats</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +146,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,19 +448,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added local currency to USD conversion for comparison purposes
</commit_message>
<xml_diff>
--- a/reports/active_assets/templates/xlsx/template.xlsx
+++ b/reports/active_assets/templates/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idigon/Repos/adobe_connect_reports/reports/active_assets/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F449CF8-2CD8-E048-ADE9-EFBF944F8DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D235F1-6C77-F245-92AB-014BB2A9F512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Asset Status</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>Seats</t>
+  </si>
+  <si>
+    <t>USD Cost</t>
+  </si>
+  <si>
+    <t>USD MSRP</t>
+  </si>
+  <si>
+    <t>USD Reseller Cost</t>
   </si>
 </sst>
 </file>
@@ -449,15 +458,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -540,13 +549,22 @@
         <v>26</v>
       </c>
       <c r="AB1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
       </c>
       <c r="AD1" t="s">
         <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>